<commit_message>
update for diynamic add form input
</commit_message>
<xml_diff>
--- a/DB_Design.xlsx
+++ b/DB_Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/my_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{567F8801-1569-974A-B1F1-DC4F680FACB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6058B1-C46A-504A-BD6A-820C0E832A97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1400" yWindow="1260" windowWidth="26060" windowHeight="19180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="189">
   <si>
     <t>No</t>
   </si>
@@ -597,6 +597,28 @@
   <si>
     <t>P/O Header</t>
   </si>
+  <si>
+    <t>total_qty</t>
+  </si>
+  <si>
+    <t>total_amount</t>
+  </si>
+  <si>
+    <t>vat</t>
+  </si>
+  <si>
+    <t>final_amount</t>
+  </si>
+  <si>
+    <t>discount_value</t>
+  </si>
+  <si>
+    <t>discount_type</t>
+  </si>
+  <si>
+    <t>0: money
+1: %</t>
+  </si>
 </sst>
 </file>
 
@@ -1141,7 +1163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1423,26 +1445,38 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1456,19 +1490,8 @@
     <xf numFmtId="49" fontId="18" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1803,14 +1826,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="137" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
@@ -32414,11 +32437,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB1075"/>
+  <dimension ref="A1:AB1082"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C104" sqref="C104"/>
+      <pane ySplit="3" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
@@ -32440,35 +32463,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="18" x14ac:dyDescent="0.15">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="152" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="148"/>
-      <c r="G1" s="149" t="s">
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
+      <c r="E1" s="153"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="155" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="147"/>
-      <c r="I1" s="147"/>
-      <c r="J1" s="147"/>
-      <c r="K1" s="147"/>
-      <c r="L1" s="147"/>
-      <c r="M1" s="147"/>
-      <c r="N1" s="147"/>
-      <c r="O1" s="148"/>
+      <c r="H1" s="153"/>
+      <c r="I1" s="153"/>
+      <c r="J1" s="153"/>
+      <c r="K1" s="153"/>
+      <c r="L1" s="153"/>
+      <c r="M1" s="153"/>
+      <c r="N1" s="153"/>
+      <c r="O1" s="154"/>
       <c r="P1" s="98"/>
       <c r="Q1" s="14"/>
-      <c r="R1" s="142" t="s">
+      <c r="R1" s="147" t="s">
         <v>43</v>
       </c>
-      <c r="S1" s="143"/>
-      <c r="T1" s="143"/>
-      <c r="U1" s="143"/>
-      <c r="V1" s="143"/>
-      <c r="W1" s="143"/>
+      <c r="S1" s="148"/>
+      <c r="T1" s="148"/>
+      <c r="U1" s="148"/>
+      <c r="V1" s="148"/>
+      <c r="W1" s="148"/>
       <c r="X1" s="14"/>
       <c r="Y1" s="14"/>
       <c r="Z1" s="14"/>
@@ -32538,16 +32561,16 @@
       <c r="AB2" s="16"/>
     </row>
     <row r="3" spans="1:28" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="144" t="s">
+      <c r="A3" s="149" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="138"/>
-      <c r="C3" s="139"/>
-      <c r="D3" s="145" t="s">
+      <c r="B3" s="140"/>
+      <c r="C3" s="141"/>
+      <c r="D3" s="151" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="138"/>
-      <c r="F3" s="139"/>
+      <c r="E3" s="140"/>
+      <c r="F3" s="141"/>
       <c r="G3" s="17"/>
       <c r="H3" s="18"/>
       <c r="I3" s="19"/>
@@ -32572,16 +32595,16 @@
       <c r="AB3" s="12"/>
     </row>
     <row r="4" spans="1:28" ht="21" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="137" t="s">
+      <c r="A4" s="144" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="138"/>
-      <c r="C4" s="139"/>
-      <c r="D4" s="141" t="s">
+      <c r="B4" s="140"/>
+      <c r="C4" s="141"/>
+      <c r="D4" s="150" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="138"/>
-      <c r="F4" s="139"/>
+      <c r="E4" s="140"/>
+      <c r="F4" s="141"/>
       <c r="G4" s="22"/>
       <c r="H4" s="22"/>
       <c r="I4" s="19"/>
@@ -33202,16 +33225,16 @@
       <c r="AB19" s="12"/>
     </row>
     <row r="20" spans="1:28" ht="21" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="150" t="s">
+      <c r="A20" s="139" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="138"/>
-      <c r="C20" s="139"/>
-      <c r="D20" s="151" t="s">
+      <c r="B20" s="140"/>
+      <c r="C20" s="141"/>
+      <c r="D20" s="142" t="s">
         <v>133</v>
       </c>
-      <c r="E20" s="138"/>
-      <c r="F20" s="139"/>
+      <c r="E20" s="140"/>
+      <c r="F20" s="141"/>
       <c r="G20" s="22"/>
       <c r="H20" s="22"/>
       <c r="I20" s="19"/>
@@ -33972,16 +33995,16 @@
       <c r="AB39" s="12"/>
     </row>
     <row r="40" spans="1:28" s="70" customFormat="1" ht="21" customHeight="1" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="150" t="s">
+      <c r="A40" s="139" t="s">
         <v>111</v>
       </c>
-      <c r="B40" s="138"/>
-      <c r="C40" s="139"/>
-      <c r="D40" s="152" t="s">
+      <c r="B40" s="140"/>
+      <c r="C40" s="141"/>
+      <c r="D40" s="143" t="s">
         <v>112</v>
       </c>
-      <c r="E40" s="138"/>
-      <c r="F40" s="139"/>
+      <c r="E40" s="140"/>
+      <c r="F40" s="141"/>
       <c r="G40" s="66"/>
       <c r="H40" s="66"/>
       <c r="I40" s="65"/>
@@ -34480,16 +34503,16 @@
       <c r="P53" s="64"/>
     </row>
     <row r="54" spans="1:28" ht="21" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="137" t="s">
+      <c r="A54" s="144" t="s">
         <v>104</v>
       </c>
-      <c r="B54" s="138"/>
-      <c r="C54" s="139"/>
-      <c r="D54" s="151" t="s">
+      <c r="B54" s="140"/>
+      <c r="C54" s="141"/>
+      <c r="D54" s="142" t="s">
         <v>110</v>
       </c>
-      <c r="E54" s="153"/>
-      <c r="F54" s="154"/>
+      <c r="E54" s="145"/>
+      <c r="F54" s="146"/>
       <c r="G54" s="22"/>
       <c r="H54" s="22"/>
       <c r="I54" s="19"/>
@@ -34838,16 +34861,16 @@
       <c r="P63" s="64"/>
     </row>
     <row r="64" spans="1:28" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="137" t="s">
+      <c r="A64" s="144" t="s">
         <v>134</v>
       </c>
-      <c r="B64" s="138"/>
-      <c r="C64" s="139"/>
-      <c r="D64" s="140" t="s">
+      <c r="B64" s="140"/>
+      <c r="C64" s="141"/>
+      <c r="D64" s="156" t="s">
         <v>181</v>
       </c>
-      <c r="E64" s="138"/>
-      <c r="F64" s="139"/>
+      <c r="E64" s="140"/>
+      <c r="F64" s="141"/>
       <c r="G64" s="22"/>
       <c r="H64" s="22"/>
       <c r="I64" s="65"/>
@@ -35409,18 +35432,16 @@
       <c r="AA79" s="12"/>
       <c r="AB79" s="12"/>
     </row>
-    <row r="80" spans="1:28" s="76" customFormat="1" ht="87" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:28" s="135" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A80" s="84"/>
       <c r="B80" s="85"/>
       <c r="C80" s="74" t="s">
-        <v>152</v>
+        <v>182</v>
       </c>
       <c r="D80" s="73" t="s">
-        <v>54</v>
-      </c>
-      <c r="E80" s="132" t="s">
-        <v>154</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="E80" s="132"/>
       <c r="F80" s="86"/>
       <c r="G80" s="77"/>
       <c r="H80" s="80"/>
@@ -35445,12 +35466,16 @@
       <c r="AA80" s="12"/>
       <c r="AB80" s="12"/>
     </row>
-    <row r="81" spans="1:28" ht="29" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:28" s="135" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A81" s="84"/>
       <c r="B81" s="85"/>
-      <c r="C81" s="74"/>
-      <c r="D81" s="73"/>
-      <c r="E81" s="73"/>
+      <c r="C81" s="74" t="s">
+        <v>183</v>
+      </c>
+      <c r="D81" s="73" t="s">
+        <v>144</v>
+      </c>
+      <c r="E81" s="132"/>
       <c r="F81" s="86"/>
       <c r="G81" s="77"/>
       <c r="H81" s="80"/>
@@ -35462,56 +35487,64 @@
       <c r="N81" s="39"/>
       <c r="O81" s="13"/>
       <c r="P81" s="31"/>
-    </row>
-    <row r="82" spans="1:28" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="137" t="s">
-        <v>135</v>
-      </c>
-      <c r="B82" s="138"/>
-      <c r="C82" s="139"/>
-      <c r="D82" s="141" t="s">
-        <v>136</v>
-      </c>
-      <c r="E82" s="138"/>
-      <c r="F82" s="139"/>
-      <c r="G82" s="22"/>
-      <c r="H82" s="22"/>
-      <c r="I82" s="65"/>
-      <c r="J82" s="65"/>
-      <c r="K82" s="65"/>
-      <c r="L82" s="65"/>
-      <c r="M82" s="65"/>
-      <c r="N82" s="65"/>
-      <c r="O82" s="66"/>
-      <c r="P82" s="67"/>
+      <c r="Q81" s="21"/>
+      <c r="R81" s="13"/>
+      <c r="S81" s="13"/>
+      <c r="T81" s="13"/>
+      <c r="U81" s="13"/>
+      <c r="V81" s="13"/>
+      <c r="W81" s="13"/>
+      <c r="X81" s="12"/>
+      <c r="Y81" s="12"/>
+      <c r="Z81" s="12"/>
+      <c r="AA81" s="12"/>
+      <c r="AB81" s="12"/>
+    </row>
+    <row r="82" spans="1:28" s="135" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="84"/>
+      <c r="B82" s="85"/>
+      <c r="C82" s="74" t="s">
+        <v>186</v>
+      </c>
+      <c r="D82" s="73" t="s">
+        <v>144</v>
+      </c>
+      <c r="E82" s="132"/>
+      <c r="F82" s="86"/>
+      <c r="G82" s="77"/>
+      <c r="H82" s="80"/>
+      <c r="I82" s="39"/>
+      <c r="J82" s="39"/>
+      <c r="K82" s="39"/>
+      <c r="L82" s="39"/>
+      <c r="M82" s="39"/>
+      <c r="N82" s="39"/>
+      <c r="O82" s="13"/>
+      <c r="P82" s="31"/>
       <c r="Q82" s="21"/>
-      <c r="R82" s="12"/>
-      <c r="S82" s="12"/>
-      <c r="T82" s="12"/>
-      <c r="U82" s="12"/>
-      <c r="V82" s="12"/>
-      <c r="W82" s="12"/>
+      <c r="R82" s="13"/>
+      <c r="S82" s="13"/>
+      <c r="T82" s="13"/>
+      <c r="U82" s="13"/>
+      <c r="V82" s="13"/>
+      <c r="W82" s="13"/>
       <c r="X82" s="12"/>
       <c r="Y82" s="12"/>
       <c r="Z82" s="12"/>
       <c r="AA82" s="12"/>
       <c r="AB82" s="12"/>
     </row>
-    <row r="83" spans="1:28" ht="29" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="84">
-        <v>1</v>
-      </c>
-      <c r="B83" s="85" t="s">
-        <v>46</v>
-      </c>
+    <row r="83" spans="1:28" s="135" customFormat="1" ht="36" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="84"/>
+      <c r="B83" s="85"/>
       <c r="C83" s="74" t="s">
-        <v>47</v>
+        <v>187</v>
       </c>
       <c r="D83" s="73" t="s">
-        <v>48</v>
-      </c>
-      <c r="E83" s="73" t="s">
-        <v>49</v>
+        <v>54</v>
+      </c>
+      <c r="E83" s="132" t="s">
+        <v>188</v>
       </c>
       <c r="F83" s="86"/>
       <c r="G83" s="77"/>
@@ -35525,9 +35558,7 @@
       <c r="O83" s="13"/>
       <c r="P83" s="31"/>
       <c r="Q83" s="21"/>
-      <c r="R83" s="13" t="s">
-        <v>56</v>
-      </c>
+      <c r="R83" s="13"/>
       <c r="S83" s="13"/>
       <c r="T83" s="13"/>
       <c r="U83" s="13"/>
@@ -35539,20 +35570,16 @@
       <c r="AA83" s="12"/>
       <c r="AB83" s="12"/>
     </row>
-    <row r="84" spans="1:28" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="84">
-        <v>2</v>
-      </c>
+    <row r="84" spans="1:28" s="135" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="84"/>
       <c r="B84" s="85"/>
       <c r="C84" s="74" t="s">
-        <v>97</v>
+        <v>184</v>
       </c>
       <c r="D84" s="73" t="s">
-        <v>54</v>
-      </c>
-      <c r="E84" s="83" t="s">
-        <v>55</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="E84" s="132"/>
       <c r="F84" s="86"/>
       <c r="G84" s="77"/>
       <c r="H84" s="80"/>
@@ -35577,20 +35604,16 @@
       <c r="AA84" s="12"/>
       <c r="AB84" s="12"/>
     </row>
-    <row r="85" spans="1:28" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="84">
-        <v>3</v>
-      </c>
+    <row r="85" spans="1:28" s="135" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="84"/>
       <c r="B85" s="85"/>
       <c r="C85" s="74" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="D85" s="73" t="s">
-        <v>54</v>
-      </c>
-      <c r="E85" s="83" t="s">
-        <v>55</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="E85" s="132"/>
       <c r="F85" s="86"/>
       <c r="G85" s="77"/>
       <c r="H85" s="80"/>
@@ -35615,20 +35638,16 @@
       <c r="AA85" s="12"/>
       <c r="AB85" s="12"/>
     </row>
-    <row r="86" spans="1:28" s="76" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="84">
-        <v>4</v>
-      </c>
+    <row r="86" spans="1:28" s="135" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="84"/>
       <c r="B86" s="85"/>
       <c r="C86" s="74" t="s">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="D86" s="73" t="s">
-        <v>54</v>
-      </c>
-      <c r="E86" s="83" t="s">
-        <v>55</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="E86" s="132"/>
       <c r="F86" s="86"/>
       <c r="G86" s="77"/>
       <c r="H86" s="80"/>
@@ -35653,19 +35672,17 @@
       <c r="AA86" s="12"/>
       <c r="AB86" s="12"/>
     </row>
-    <row r="87" spans="1:28" s="133" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="84">
-        <v>5</v>
-      </c>
+    <row r="87" spans="1:28" s="76" customFormat="1" ht="87" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="84"/>
       <c r="B87" s="85"/>
       <c r="C87" s="74" t="s">
-        <v>114</v>
+        <v>152</v>
       </c>
       <c r="D87" s="73" t="s">
-        <v>51</v>
-      </c>
-      <c r="E87" s="83" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="E87" s="132" t="s">
+        <v>154</v>
       </c>
       <c r="F87" s="86"/>
       <c r="G87" s="77"/>
@@ -35691,20 +35708,12 @@
       <c r="AA87" s="12"/>
       <c r="AB87" s="12"/>
     </row>
-    <row r="88" spans="1:28" s="76" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="84">
-        <v>6</v>
-      </c>
+    <row r="88" spans="1:28" ht="29" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="84"/>
       <c r="B88" s="85"/>
-      <c r="C88" s="74" t="s">
-        <v>143</v>
-      </c>
-      <c r="D88" s="73" t="s">
-        <v>144</v>
-      </c>
-      <c r="E88" s="83" t="s">
-        <v>55</v>
-      </c>
+      <c r="C88" s="74"/>
+      <c r="D88" s="73"/>
+      <c r="E88" s="73"/>
       <c r="F88" s="86"/>
       <c r="G88" s="77"/>
       <c r="H88" s="80"/>
@@ -35716,70 +35725,56 @@
       <c r="N88" s="39"/>
       <c r="O88" s="13"/>
       <c r="P88" s="31"/>
-      <c r="Q88" s="21"/>
-      <c r="R88" s="13"/>
-      <c r="S88" s="13"/>
-      <c r="T88" s="13"/>
-      <c r="U88" s="13"/>
-      <c r="V88" s="13"/>
-      <c r="W88" s="13"/>
-      <c r="X88" s="12"/>
-      <c r="Y88" s="12"/>
-      <c r="Z88" s="12"/>
-      <c r="AA88" s="12"/>
-      <c r="AB88" s="12"/>
-    </row>
-    <row r="89" spans="1:28" s="76" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="84">
-        <v>7</v>
-      </c>
-      <c r="B89" s="85"/>
-      <c r="C89" s="74" t="s">
-        <v>115</v>
-      </c>
-      <c r="D89" s="73" t="s">
-        <v>54</v>
-      </c>
-      <c r="E89" s="83" t="s">
-        <v>55</v>
-      </c>
-      <c r="F89" s="86"/>
-      <c r="G89" s="77"/>
-      <c r="H89" s="80"/>
-      <c r="I89" s="39"/>
-      <c r="J89" s="39"/>
-      <c r="K89" s="39"/>
-      <c r="L89" s="39"/>
-      <c r="M89" s="39"/>
-      <c r="N89" s="39"/>
-      <c r="O89" s="13"/>
-      <c r="P89" s="31"/>
+    </row>
+    <row r="89" spans="1:28" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="144" t="s">
+        <v>135</v>
+      </c>
+      <c r="B89" s="140"/>
+      <c r="C89" s="141"/>
+      <c r="D89" s="150" t="s">
+        <v>136</v>
+      </c>
+      <c r="E89" s="140"/>
+      <c r="F89" s="141"/>
+      <c r="G89" s="22"/>
+      <c r="H89" s="22"/>
+      <c r="I89" s="65"/>
+      <c r="J89" s="65"/>
+      <c r="K89" s="65"/>
+      <c r="L89" s="65"/>
+      <c r="M89" s="65"/>
+      <c r="N89" s="65"/>
+      <c r="O89" s="66"/>
+      <c r="P89" s="67"/>
       <c r="Q89" s="21"/>
-      <c r="R89" s="13"/>
-      <c r="S89" s="13"/>
-      <c r="T89" s="13"/>
-      <c r="U89" s="13"/>
-      <c r="V89" s="13"/>
-      <c r="W89" s="13"/>
+      <c r="R89" s="12"/>
+      <c r="S89" s="12"/>
+      <c r="T89" s="12"/>
+      <c r="U89" s="12"/>
+      <c r="V89" s="12"/>
+      <c r="W89" s="12"/>
       <c r="X89" s="12"/>
       <c r="Y89" s="12"/>
       <c r="Z89" s="12"/>
       <c r="AA89" s="12"/>
       <c r="AB89" s="12"/>
     </row>
-    <row r="90" spans="1:28" s="76" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:28" ht="29" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A90" s="84">
-        <v>8</v>
-      </c>
-      <c r="B90" s="85"/>
+        <v>1</v>
+      </c>
+      <c r="B90" s="85" t="s">
+        <v>46</v>
+      </c>
       <c r="C90" s="74" t="s">
-        <v>146</v>
+        <v>47</v>
       </c>
       <c r="D90" s="73" t="s">
-        <v>144</v>
-      </c>
-      <c r="E90" s="83" t="s">
-        <v>55</v>
+        <v>48</v>
+      </c>
+      <c r="E90" s="73" t="s">
+        <v>49</v>
       </c>
       <c r="F90" s="86"/>
       <c r="G90" s="77"/>
@@ -35793,7 +35788,9 @@
       <c r="O90" s="13"/>
       <c r="P90" s="31"/>
       <c r="Q90" s="21"/>
-      <c r="R90" s="13"/>
+      <c r="R90" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="S90" s="13"/>
       <c r="T90" s="13"/>
       <c r="U90" s="13"/>
@@ -35805,16 +35802,16 @@
       <c r="AA90" s="12"/>
       <c r="AB90" s="12"/>
     </row>
-    <row r="91" spans="1:28" s="76" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:28" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A91" s="84">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B91" s="85"/>
       <c r="C91" s="74" t="s">
-        <v>145</v>
+        <v>97</v>
       </c>
       <c r="D91" s="73" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="E91" s="83" t="s">
         <v>55</v>
@@ -35843,23 +35840,21 @@
       <c r="AA91" s="12"/>
       <c r="AB91" s="12"/>
     </row>
-    <row r="92" spans="1:28" s="76" customFormat="1" ht="42" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:28" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A92" s="84">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B92" s="85"/>
       <c r="C92" s="74" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="D92" s="73" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="E92" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="F92" s="130" t="s">
-        <v>148</v>
-      </c>
+      <c r="F92" s="86"/>
       <c r="G92" s="77"/>
       <c r="H92" s="80"/>
       <c r="I92" s="39"/>
@@ -35883,28 +35878,24 @@
       <c r="AA92" s="12"/>
       <c r="AB92" s="12"/>
     </row>
-    <row r="93" spans="1:28" s="76" customFormat="1" ht="42" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:28" s="76" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A93" s="84">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B93" s="85"/>
       <c r="C93" s="74" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D93" s="73" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="E93" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="F93" s="130" t="s">
-        <v>151</v>
-      </c>
+      <c r="F93" s="86"/>
       <c r="G93" s="77"/>
       <c r="H93" s="80"/>
-      <c r="I93" s="130" t="s">
-        <v>150</v>
-      </c>
+      <c r="I93" s="39"/>
       <c r="J93" s="39"/>
       <c r="K93" s="39"/>
       <c r="L93" s="39"/>
@@ -35925,23 +35916,21 @@
       <c r="AA93" s="12"/>
       <c r="AB93" s="12"/>
     </row>
-    <row r="94" spans="1:28" ht="84" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:28" s="133" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A94" s="84">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B94" s="85"/>
       <c r="C94" s="74" t="s">
-        <v>152</v>
+        <v>114</v>
       </c>
       <c r="D94" s="73" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E94" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="F94" s="130" t="s">
-        <v>153</v>
-      </c>
+      <c r="F94" s="86"/>
       <c r="G94" s="77"/>
       <c r="H94" s="80"/>
       <c r="I94" s="39"/>
@@ -35965,12 +35954,20 @@
       <c r="AA94" s="12"/>
       <c r="AB94" s="12"/>
     </row>
-    <row r="95" spans="1:28" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="84"/>
+    <row r="95" spans="1:28" s="76" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="84">
+        <v>6</v>
+      </c>
       <c r="B95" s="85"/>
-      <c r="C95" s="74"/>
-      <c r="D95" s="73"/>
-      <c r="E95" s="73"/>
+      <c r="C95" s="74" t="s">
+        <v>143</v>
+      </c>
+      <c r="D95" s="73" t="s">
+        <v>144</v>
+      </c>
+      <c r="E95" s="83" t="s">
+        <v>55</v>
+      </c>
       <c r="F95" s="86"/>
       <c r="G95" s="77"/>
       <c r="H95" s="80"/>
@@ -35995,12 +35992,20 @@
       <c r="AA95" s="12"/>
       <c r="AB95" s="12"/>
     </row>
-    <row r="96" spans="1:28" ht="29" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="84"/>
+    <row r="96" spans="1:28" s="76" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="84">
+        <v>7</v>
+      </c>
       <c r="B96" s="85"/>
-      <c r="C96" s="74"/>
-      <c r="D96" s="73"/>
-      <c r="E96" s="73"/>
+      <c r="C96" s="74" t="s">
+        <v>115</v>
+      </c>
+      <c r="D96" s="73" t="s">
+        <v>54</v>
+      </c>
+      <c r="E96" s="83" t="s">
+        <v>55</v>
+      </c>
       <c r="F96" s="86"/>
       <c r="G96" s="77"/>
       <c r="H96" s="80"/>
@@ -36012,76 +36017,84 @@
       <c r="N96" s="39"/>
       <c r="O96" s="13"/>
       <c r="P96" s="31"/>
-    </row>
-    <row r="97" spans="1:28" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="137" t="s">
-        <v>137</v>
-      </c>
-      <c r="B97" s="138"/>
-      <c r="C97" s="139"/>
-      <c r="D97" s="140" t="s">
-        <v>138</v>
-      </c>
-      <c r="E97" s="138"/>
-      <c r="F97" s="139"/>
-      <c r="G97" s="22"/>
-      <c r="H97" s="22"/>
-      <c r="I97" s="65"/>
-      <c r="J97" s="65"/>
-      <c r="K97" s="65"/>
-      <c r="L97" s="65"/>
-      <c r="M97" s="65"/>
-      <c r="N97" s="65"/>
-      <c r="O97" s="66"/>
-      <c r="P97" s="67"/>
+      <c r="Q96" s="21"/>
+      <c r="R96" s="13"/>
+      <c r="S96" s="13"/>
+      <c r="T96" s="13"/>
+      <c r="U96" s="13"/>
+      <c r="V96" s="13"/>
+      <c r="W96" s="13"/>
+      <c r="X96" s="12"/>
+      <c r="Y96" s="12"/>
+      <c r="Z96" s="12"/>
+      <c r="AA96" s="12"/>
+      <c r="AB96" s="12"/>
+    </row>
+    <row r="97" spans="1:28" s="76" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="84">
+        <v>8</v>
+      </c>
+      <c r="B97" s="85"/>
+      <c r="C97" s="74" t="s">
+        <v>146</v>
+      </c>
+      <c r="D97" s="73" t="s">
+        <v>144</v>
+      </c>
+      <c r="E97" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="F97" s="86"/>
+      <c r="G97" s="77"/>
+      <c r="H97" s="80"/>
+      <c r="I97" s="39"/>
+      <c r="J97" s="39"/>
+      <c r="K97" s="39"/>
+      <c r="L97" s="39"/>
+      <c r="M97" s="39"/>
+      <c r="N97" s="39"/>
+      <c r="O97" s="13"/>
+      <c r="P97" s="31"/>
       <c r="Q97" s="21"/>
-      <c r="R97" s="12"/>
-      <c r="S97" s="12"/>
-      <c r="T97" s="12"/>
-      <c r="U97" s="12"/>
-      <c r="V97" s="12"/>
-      <c r="W97" s="12"/>
+      <c r="R97" s="13"/>
+      <c r="S97" s="13"/>
+      <c r="T97" s="13"/>
+      <c r="U97" s="13"/>
+      <c r="V97" s="13"/>
+      <c r="W97" s="13"/>
       <c r="X97" s="12"/>
       <c r="Y97" s="12"/>
       <c r="Z97" s="12"/>
       <c r="AA97" s="12"/>
       <c r="AB97" s="12"/>
     </row>
-    <row r="98" spans="1:28" ht="19" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:28" s="76" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A98" s="84">
-        <v>1</v>
-      </c>
-      <c r="B98" s="85" t="s">
-        <v>46</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B98" s="85"/>
       <c r="C98" s="74" t="s">
-        <v>47</v>
+        <v>145</v>
       </c>
       <c r="D98" s="73" t="s">
-        <v>48</v>
-      </c>
-      <c r="E98" s="73" t="s">
-        <v>49</v>
-      </c>
-      <c r="F98" s="29"/>
-      <c r="G98" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="H98" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="I98" s="30"/>
-      <c r="J98" s="30"/>
-      <c r="K98" s="30"/>
-      <c r="L98" s="30"/>
-      <c r="M98" s="30"/>
-      <c r="N98" s="30"/>
+        <v>144</v>
+      </c>
+      <c r="E98" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="F98" s="86"/>
+      <c r="G98" s="77"/>
+      <c r="H98" s="80"/>
+      <c r="I98" s="39"/>
+      <c r="J98" s="39"/>
+      <c r="K98" s="39"/>
+      <c r="L98" s="39"/>
+      <c r="M98" s="39"/>
+      <c r="N98" s="39"/>
       <c r="O98" s="13"/>
       <c r="P98" s="31"/>
       <c r="Q98" s="21"/>
-      <c r="R98" s="13" t="s">
-        <v>56</v>
-      </c>
+      <c r="R98" s="13"/>
       <c r="S98" s="13"/>
       <c r="T98" s="13"/>
       <c r="U98" s="13"/>
@@ -36093,21 +36106,23 @@
       <c r="AA98" s="12"/>
       <c r="AB98" s="12"/>
     </row>
-    <row r="99" spans="1:28" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:28" s="76" customFormat="1" ht="42" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A99" s="84">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B99" s="85"/>
       <c r="C99" s="74" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="D99" s="73" t="s">
-        <v>54</v>
+        <v>144</v>
       </c>
       <c r="E99" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="F99" s="86"/>
+      <c r="F99" s="130" t="s">
+        <v>148</v>
+      </c>
       <c r="G99" s="77"/>
       <c r="H99" s="80"/>
       <c r="I99" s="39"/>
@@ -36131,24 +36146,28 @@
       <c r="AA99" s="12"/>
       <c r="AB99" s="12"/>
     </row>
-    <row r="100" spans="1:28" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:28" s="76" customFormat="1" ht="42" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A100" s="84">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B100" s="85"/>
       <c r="C100" s="74" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="D100" s="73" t="s">
-        <v>54</v>
+        <v>144</v>
       </c>
       <c r="E100" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="F100" s="86"/>
+      <c r="F100" s="130" t="s">
+        <v>151</v>
+      </c>
       <c r="G100" s="77"/>
       <c r="H100" s="80"/>
-      <c r="I100" s="39"/>
+      <c r="I100" s="130" t="s">
+        <v>150</v>
+      </c>
       <c r="J100" s="39"/>
       <c r="K100" s="39"/>
       <c r="L100" s="39"/>
@@ -36169,22 +36188,22 @@
       <c r="AA100" s="12"/>
       <c r="AB100" s="12"/>
     </row>
-    <row r="101" spans="1:28" s="133" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:28" ht="84" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A101" s="84">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B101" s="85"/>
       <c r="C101" s="74" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="D101" s="73" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="E101" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="F101" s="86" t="s">
-        <v>179</v>
+      <c r="F101" s="130" t="s">
+        <v>153</v>
       </c>
       <c r="G101" s="77"/>
       <c r="H101" s="80"/>
@@ -36209,28 +36228,16 @@
       <c r="AA101" s="12"/>
       <c r="AB101" s="12"/>
     </row>
-    <row r="102" spans="1:28" s="133" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="84">
-        <v>5</v>
-      </c>
+    <row r="102" spans="1:28" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="84"/>
       <c r="B102" s="85"/>
-      <c r="C102" s="74" t="s">
-        <v>149</v>
-      </c>
-      <c r="D102" s="73" t="s">
-        <v>144</v>
-      </c>
-      <c r="E102" s="83" t="s">
-        <v>55</v>
-      </c>
-      <c r="F102" s="86" t="s">
-        <v>180</v>
-      </c>
+      <c r="C102" s="74"/>
+      <c r="D102" s="73"/>
+      <c r="E102" s="73"/>
+      <c r="F102" s="86"/>
       <c r="G102" s="77"/>
       <c r="H102" s="80"/>
-      <c r="I102" s="93" t="s">
-        <v>150</v>
-      </c>
+      <c r="I102" s="39"/>
       <c r="J102" s="39"/>
       <c r="K102" s="39"/>
       <c r="L102" s="39"/>
@@ -36251,23 +36258,13 @@
       <c r="AA102" s="12"/>
       <c r="AB102" s="12"/>
     </row>
-    <row r="103" spans="1:28" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="84">
-        <v>6</v>
-      </c>
+    <row r="103" spans="1:28" ht="29" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="84"/>
       <c r="B103" s="85"/>
-      <c r="C103" s="74" t="s">
-        <v>176</v>
-      </c>
-      <c r="D103" s="73" t="s">
-        <v>165</v>
-      </c>
-      <c r="E103" s="83" t="s">
-        <v>55</v>
-      </c>
-      <c r="F103" s="86" t="s">
-        <v>178</v>
-      </c>
+      <c r="C103" s="74"/>
+      <c r="D103" s="73"/>
+      <c r="E103" s="73"/>
+      <c r="F103" s="86"/>
       <c r="G103" s="77"/>
       <c r="H103" s="80"/>
       <c r="I103" s="39"/>
@@ -36278,78 +36275,76 @@
       <c r="N103" s="39"/>
       <c r="O103" s="13"/>
       <c r="P103" s="31"/>
-      <c r="Q103" s="21"/>
-      <c r="R103" s="13"/>
-      <c r="S103" s="13"/>
-      <c r="T103" s="13"/>
-      <c r="U103" s="13"/>
-      <c r="V103" s="13"/>
-      <c r="W103" s="13"/>
-      <c r="X103" s="12"/>
-      <c r="Y103" s="12"/>
-      <c r="Z103" s="12"/>
-      <c r="AA103" s="12"/>
-      <c r="AB103" s="12"/>
-    </row>
-    <row r="104" spans="1:28" s="133" customFormat="1" ht="84" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="84">
-        <v>7</v>
-      </c>
-      <c r="B104" s="85"/>
-      <c r="C104" s="74" t="s">
-        <v>152</v>
-      </c>
-      <c r="D104" s="73" t="s">
-        <v>54</v>
-      </c>
-      <c r="E104" s="83" t="s">
-        <v>55</v>
-      </c>
-      <c r="F104" s="155" t="s">
-        <v>177</v>
-      </c>
-      <c r="G104" s="77"/>
-      <c r="H104" s="80"/>
-      <c r="I104" s="39"/>
-      <c r="J104" s="39"/>
-      <c r="K104" s="39"/>
-      <c r="L104" s="39"/>
-      <c r="M104" s="39"/>
-      <c r="N104" s="39"/>
-      <c r="O104" s="13"/>
-      <c r="P104" s="31"/>
+    </row>
+    <row r="104" spans="1:28" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="144" t="s">
+        <v>137</v>
+      </c>
+      <c r="B104" s="140"/>
+      <c r="C104" s="141"/>
+      <c r="D104" s="156" t="s">
+        <v>138</v>
+      </c>
+      <c r="E104" s="140"/>
+      <c r="F104" s="141"/>
+      <c r="G104" s="22"/>
+      <c r="H104" s="22"/>
+      <c r="I104" s="65"/>
+      <c r="J104" s="65"/>
+      <c r="K104" s="65"/>
+      <c r="L104" s="65"/>
+      <c r="M104" s="65"/>
+      <c r="N104" s="65"/>
+      <c r="O104" s="66"/>
+      <c r="P104" s="67"/>
       <c r="Q104" s="21"/>
-      <c r="R104" s="13"/>
-      <c r="S104" s="13"/>
-      <c r="T104" s="13"/>
-      <c r="U104" s="13"/>
-      <c r="V104" s="13"/>
-      <c r="W104" s="13"/>
+      <c r="R104" s="12"/>
+      <c r="S104" s="12"/>
+      <c r="T104" s="12"/>
+      <c r="U104" s="12"/>
+      <c r="V104" s="12"/>
+      <c r="W104" s="12"/>
       <c r="X104" s="12"/>
       <c r="Y104" s="12"/>
       <c r="Z104" s="12"/>
       <c r="AA104" s="12"/>
       <c r="AB104" s="12"/>
     </row>
-    <row r="105" spans="1:28" s="133" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="84"/>
-      <c r="B105" s="85"/>
-      <c r="C105" s="74"/>
-      <c r="D105" s="73"/>
-      <c r="E105" s="83"/>
-      <c r="F105" s="86"/>
-      <c r="G105" s="77"/>
-      <c r="H105" s="80"/>
-      <c r="I105" s="39"/>
-      <c r="J105" s="39"/>
-      <c r="K105" s="39"/>
-      <c r="L105" s="39"/>
-      <c r="M105" s="39"/>
-      <c r="N105" s="39"/>
+    <row r="105" spans="1:28" ht="19" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="84">
+        <v>1</v>
+      </c>
+      <c r="B105" s="85" t="s">
+        <v>46</v>
+      </c>
+      <c r="C105" s="74" t="s">
+        <v>47</v>
+      </c>
+      <c r="D105" s="73" t="s">
+        <v>48</v>
+      </c>
+      <c r="E105" s="73" t="s">
+        <v>49</v>
+      </c>
+      <c r="F105" s="29"/>
+      <c r="G105" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="H105" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="I105" s="30"/>
+      <c r="J105" s="30"/>
+      <c r="K105" s="30"/>
+      <c r="L105" s="30"/>
+      <c r="M105" s="30"/>
+      <c r="N105" s="30"/>
       <c r="O105" s="13"/>
       <c r="P105" s="31"/>
       <c r="Q105" s="21"/>
-      <c r="R105" s="13"/>
+      <c r="R105" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="S105" s="13"/>
       <c r="T105" s="13"/>
       <c r="U105" s="13"/>
@@ -36361,96 +36356,111 @@
       <c r="AA105" s="12"/>
       <c r="AB105" s="12"/>
     </row>
-    <row r="106" spans="1:28" ht="14" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="60"/>
-      <c r="B106" s="61"/>
-      <c r="C106" s="61"/>
-      <c r="D106" s="61"/>
-      <c r="E106" s="61"/>
-      <c r="F106" s="62"/>
-      <c r="G106" s="61"/>
-      <c r="H106" s="61"/>
-      <c r="I106" s="61"/>
-      <c r="J106" s="61"/>
-      <c r="K106" s="61"/>
-      <c r="L106" s="61"/>
-      <c r="M106" s="61"/>
-      <c r="N106" s="61"/>
-      <c r="O106" s="61"/>
-      <c r="P106" s="64"/>
-    </row>
-    <row r="107" spans="1:28" ht="22.5" customHeight="1" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="137" t="s">
-        <v>139</v>
-      </c>
-      <c r="B107" s="138"/>
-      <c r="C107" s="139"/>
-      <c r="D107" s="140" t="s">
-        <v>140</v>
-      </c>
-      <c r="E107" s="138"/>
-      <c r="F107" s="139"/>
-      <c r="G107" s="22"/>
-      <c r="H107" s="22"/>
-      <c r="I107" s="65"/>
-      <c r="J107" s="65"/>
-      <c r="K107" s="65"/>
-      <c r="L107" s="65"/>
-      <c r="M107" s="65"/>
-      <c r="N107" s="65"/>
-      <c r="O107" s="66"/>
-      <c r="P107" s="67"/>
+    <row r="106" spans="1:28" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="84">
+        <v>2</v>
+      </c>
+      <c r="B106" s="85"/>
+      <c r="C106" s="74" t="s">
+        <v>175</v>
+      </c>
+      <c r="D106" s="73" t="s">
+        <v>54</v>
+      </c>
+      <c r="E106" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="F106" s="86"/>
+      <c r="G106" s="77"/>
+      <c r="H106" s="80"/>
+      <c r="I106" s="39"/>
+      <c r="J106" s="39"/>
+      <c r="K106" s="39"/>
+      <c r="L106" s="39"/>
+      <c r="M106" s="39"/>
+      <c r="N106" s="39"/>
+      <c r="O106" s="13"/>
+      <c r="P106" s="31"/>
+      <c r="Q106" s="21"/>
+      <c r="R106" s="13"/>
+      <c r="S106" s="13"/>
+      <c r="T106" s="13"/>
+      <c r="U106" s="13"/>
+      <c r="V106" s="13"/>
+      <c r="W106" s="13"/>
+      <c r="X106" s="12"/>
+      <c r="Y106" s="12"/>
+      <c r="Z106" s="12"/>
+      <c r="AA106" s="12"/>
+      <c r="AB106" s="12"/>
+    </row>
+    <row r="107" spans="1:28" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="84">
+        <v>3</v>
+      </c>
+      <c r="B107" s="85"/>
+      <c r="C107" s="74" t="s">
+        <v>174</v>
+      </c>
+      <c r="D107" s="73" t="s">
+        <v>54</v>
+      </c>
+      <c r="E107" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="F107" s="86"/>
+      <c r="G107" s="77"/>
+      <c r="H107" s="80"/>
+      <c r="I107" s="39"/>
+      <c r="J107" s="39"/>
+      <c r="K107" s="39"/>
+      <c r="L107" s="39"/>
+      <c r="M107" s="39"/>
+      <c r="N107" s="39"/>
+      <c r="O107" s="13"/>
+      <c r="P107" s="31"/>
       <c r="Q107" s="21"/>
-      <c r="R107" s="12"/>
-      <c r="S107" s="12"/>
-      <c r="T107" s="12"/>
-      <c r="U107" s="12"/>
-      <c r="V107" s="12"/>
-      <c r="W107" s="12"/>
+      <c r="R107" s="13"/>
+      <c r="S107" s="13"/>
+      <c r="T107" s="13"/>
+      <c r="U107" s="13"/>
+      <c r="V107" s="13"/>
+      <c r="W107" s="13"/>
       <c r="X107" s="12"/>
       <c r="Y107" s="12"/>
       <c r="Z107" s="12"/>
       <c r="AA107" s="12"/>
       <c r="AB107" s="12"/>
     </row>
-    <row r="108" spans="1:28" ht="19" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="25">
-        <v>1</v>
-      </c>
-      <c r="B108" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C108" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="D108" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="E108" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="F108" s="29" t="e">
-        <f>IF(OR(H108 = "", H108 = "ー", H108 = "-"), "", LOWER(H108) &amp; IF(N108 &lt;&gt; "", ":" &amp; N108 &amp; "|", "|") &amp; IF(O108 &lt;&gt; "", "search|", "")) &amp; "ja:" &amp;#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G108" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="H108" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="I108" s="30"/>
-      <c r="J108" s="30"/>
-      <c r="K108" s="30"/>
-      <c r="L108" s="30"/>
-      <c r="M108" s="30"/>
-      <c r="N108" s="30"/>
+    <row r="108" spans="1:28" s="133" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="84">
+        <v>4</v>
+      </c>
+      <c r="B108" s="85"/>
+      <c r="C108" s="74" t="s">
+        <v>143</v>
+      </c>
+      <c r="D108" s="73" t="s">
+        <v>144</v>
+      </c>
+      <c r="E108" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="F108" s="86" t="s">
+        <v>179</v>
+      </c>
+      <c r="G108" s="77"/>
+      <c r="H108" s="80"/>
+      <c r="I108" s="39"/>
+      <c r="J108" s="39"/>
+      <c r="K108" s="39"/>
+      <c r="L108" s="39"/>
+      <c r="M108" s="39"/>
+      <c r="N108" s="39"/>
       <c r="O108" s="13"/>
       <c r="P108" s="31"/>
       <c r="Q108" s="21"/>
-      <c r="R108" s="13" t="s">
-        <v>56</v>
-      </c>
+      <c r="R108" s="13"/>
       <c r="S108" s="13"/>
       <c r="T108" s="13"/>
       <c r="U108" s="13"/>
@@ -36462,28 +36472,35 @@
       <c r="AA108" s="12"/>
       <c r="AB108" s="12"/>
     </row>
-    <row r="109" spans="1:28" ht="18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="47">
-        <v>2</v>
-      </c>
-      <c r="B109" s="26"/>
-      <c r="C109" s="33"/>
-      <c r="D109" s="34"/>
-      <c r="E109" s="38"/>
-      <c r="F109" s="29" t="e">
-        <f>IF(OR(H109 = "", H109 = "ー", H109 = "-"), "", LOWER(H109) &amp; IF(N109 &lt;&gt; "", ":" &amp; N109 &amp; "|", "|") &amp; IF(O109 &lt;&gt; "", "search|", "")) &amp; "ja:" &amp;#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G109" s="28"/>
-      <c r="H109" s="30"/>
-      <c r="I109" s="30"/>
-      <c r="J109" s="30"/>
-      <c r="K109" s="30"/>
-      <c r="L109" s="30"/>
-      <c r="M109" s="30"/>
-      <c r="N109" s="30"/>
-      <c r="O109" s="28"/>
-      <c r="P109" s="36"/>
+    <row r="109" spans="1:28" s="133" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="84">
+        <v>5</v>
+      </c>
+      <c r="B109" s="85"/>
+      <c r="C109" s="74" t="s">
+        <v>149</v>
+      </c>
+      <c r="D109" s="73" t="s">
+        <v>144</v>
+      </c>
+      <c r="E109" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="F109" s="86" t="s">
+        <v>180</v>
+      </c>
+      <c r="G109" s="77"/>
+      <c r="H109" s="80"/>
+      <c r="I109" s="93" t="s">
+        <v>150</v>
+      </c>
+      <c r="J109" s="39"/>
+      <c r="K109" s="39"/>
+      <c r="L109" s="39"/>
+      <c r="M109" s="39"/>
+      <c r="N109" s="39"/>
+      <c r="O109" s="13"/>
+      <c r="P109" s="31"/>
       <c r="Q109" s="21"/>
       <c r="R109" s="13"/>
       <c r="S109" s="13"/>
@@ -36497,28 +36514,33 @@
       <c r="AA109" s="12"/>
       <c r="AB109" s="12"/>
     </row>
-    <row r="110" spans="1:28" ht="18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="47">
-        <v>3</v>
-      </c>
-      <c r="B110" s="26"/>
-      <c r="C110" s="33"/>
-      <c r="D110" s="34"/>
-      <c r="E110" s="38"/>
-      <c r="F110" s="29" t="e">
-        <f>IF(OR(H110 = "", H110 = "ー", H110 = "-"), "", LOWER(H110) &amp; IF(N110 &lt;&gt; "", ":" &amp; N110 &amp; "|", "|") &amp; IF(O110 &lt;&gt; "", "search|", "")) &amp; "ja:" &amp;#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G110" s="28"/>
-      <c r="H110" s="30"/>
-      <c r="I110" s="30"/>
-      <c r="J110" s="30"/>
-      <c r="K110" s="30"/>
-      <c r="L110" s="30"/>
-      <c r="M110" s="30"/>
-      <c r="N110" s="30"/>
-      <c r="O110" s="28"/>
-      <c r="P110" s="36"/>
+    <row r="110" spans="1:28" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="84">
+        <v>6</v>
+      </c>
+      <c r="B110" s="85"/>
+      <c r="C110" s="74" t="s">
+        <v>176</v>
+      </c>
+      <c r="D110" s="73" t="s">
+        <v>165</v>
+      </c>
+      <c r="E110" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="F110" s="86" t="s">
+        <v>178</v>
+      </c>
+      <c r="G110" s="77"/>
+      <c r="H110" s="80"/>
+      <c r="I110" s="39"/>
+      <c r="J110" s="39"/>
+      <c r="K110" s="39"/>
+      <c r="L110" s="39"/>
+      <c r="M110" s="39"/>
+      <c r="N110" s="39"/>
+      <c r="O110" s="13"/>
+      <c r="P110" s="31"/>
       <c r="Q110" s="21"/>
       <c r="R110" s="13"/>
       <c r="S110" s="13"/>
@@ -36532,28 +36554,33 @@
       <c r="AA110" s="12"/>
       <c r="AB110" s="12"/>
     </row>
-    <row r="111" spans="1:28" ht="18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="47">
-        <v>4</v>
-      </c>
-      <c r="B111" s="26"/>
-      <c r="C111" s="33"/>
-      <c r="D111" s="34"/>
-      <c r="E111" s="38"/>
-      <c r="F111" s="29" t="e">
-        <f>IF(OR(H111 = "", H111 = "ー", H111 = "-"), "", LOWER(H111) &amp; IF(N111 &lt;&gt; "", ":" &amp; N111 &amp; "|", "|") &amp; IF(O111 &lt;&gt; "", "search|", "")) &amp; "ja:" &amp;#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G111" s="28"/>
-      <c r="H111" s="30"/>
-      <c r="I111" s="48"/>
-      <c r="J111" s="48"/>
-      <c r="K111" s="48"/>
-      <c r="L111" s="48"/>
-      <c r="M111" s="48"/>
-      <c r="N111" s="48"/>
-      <c r="O111" s="28"/>
-      <c r="P111" s="36"/>
+    <row r="111" spans="1:28" s="133" customFormat="1" ht="84" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="84">
+        <v>7</v>
+      </c>
+      <c r="B111" s="85"/>
+      <c r="C111" s="74" t="s">
+        <v>152</v>
+      </c>
+      <c r="D111" s="73" t="s">
+        <v>54</v>
+      </c>
+      <c r="E111" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="F111" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="G111" s="77"/>
+      <c r="H111" s="80"/>
+      <c r="I111" s="39"/>
+      <c r="J111" s="39"/>
+      <c r="K111" s="39"/>
+      <c r="L111" s="39"/>
+      <c r="M111" s="39"/>
+      <c r="N111" s="39"/>
+      <c r="O111" s="13"/>
+      <c r="P111" s="31"/>
       <c r="Q111" s="21"/>
       <c r="R111" s="13"/>
       <c r="S111" s="13"/>
@@ -36567,26 +36594,23 @@
       <c r="AA111" s="12"/>
       <c r="AB111" s="12"/>
     </row>
-    <row r="112" spans="1:28" ht="18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="25"/>
-      <c r="B112" s="26"/>
-      <c r="C112" s="49"/>
-      <c r="D112" s="28"/>
-      <c r="E112" s="34"/>
-      <c r="F112" s="29" t="e">
-        <f>IF(OR(H112 = "", H112 = "ー", H112 = "-"), "", LOWER(H112) &amp; IF(N112 &lt;&gt; "", ":" &amp; N112 &amp; "|", "|") &amp; IF(O112 &lt;&gt; "", "search|", "")) &amp; "ja:" &amp;#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G112" s="28"/>
-      <c r="H112" s="30"/>
-      <c r="I112" s="30"/>
-      <c r="J112" s="30"/>
-      <c r="K112" s="30"/>
-      <c r="L112" s="30"/>
-      <c r="M112" s="30"/>
-      <c r="N112" s="30"/>
+    <row r="112" spans="1:28" s="133" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="84"/>
+      <c r="B112" s="85"/>
+      <c r="C112" s="74"/>
+      <c r="D112" s="73"/>
+      <c r="E112" s="83"/>
+      <c r="F112" s="86"/>
+      <c r="G112" s="77"/>
+      <c r="H112" s="80"/>
+      <c r="I112" s="39"/>
+      <c r="J112" s="39"/>
+      <c r="K112" s="39"/>
+      <c r="L112" s="39"/>
+      <c r="M112" s="39"/>
+      <c r="N112" s="39"/>
       <c r="O112" s="13"/>
-      <c r="P112" s="36"/>
+      <c r="P112" s="31"/>
       <c r="Q112" s="21"/>
       <c r="R112" s="13"/>
       <c r="S112" s="13"/>
@@ -36600,7 +36624,7 @@
       <c r="AA112" s="12"/>
       <c r="AB112" s="12"/>
     </row>
-    <row r="113" spans="1:28" ht="14" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:28" ht="14" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A113" s="60"/>
       <c r="B113" s="61"/>
       <c r="C113" s="61"/>
@@ -36618,19 +36642,19 @@
       <c r="O113" s="61"/>
       <c r="P113" s="64"/>
     </row>
-    <row r="114" spans="1:28" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="137" t="s">
-        <v>155</v>
-      </c>
-      <c r="B114" s="138"/>
-      <c r="C114" s="139"/>
-      <c r="D114" s="140" t="s">
-        <v>156</v>
-      </c>
-      <c r="E114" s="138"/>
-      <c r="F114" s="139"/>
-      <c r="G114" s="66"/>
-      <c r="H114" s="66"/>
+    <row r="114" spans="1:28" ht="22.5" customHeight="1" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="144" t="s">
+        <v>139</v>
+      </c>
+      <c r="B114" s="140"/>
+      <c r="C114" s="141"/>
+      <c r="D114" s="156" t="s">
+        <v>140</v>
+      </c>
+      <c r="E114" s="140"/>
+      <c r="F114" s="141"/>
+      <c r="G114" s="22"/>
+      <c r="H114" s="22"/>
       <c r="I114" s="65"/>
       <c r="J114" s="65"/>
       <c r="K114" s="65"/>
@@ -36652,31 +36676,38 @@
       <c r="AA114" s="12"/>
       <c r="AB114" s="12"/>
     </row>
-    <row r="115" spans="1:28" ht="29" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="84">
+    <row r="115" spans="1:28" ht="19" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="25">
         <v>1</v>
       </c>
-      <c r="B115" s="85" t="s">
+      <c r="B115" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="C115" s="74" t="s">
+      <c r="C115" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="D115" s="73" t="s">
+      <c r="D115" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="E115" s="83" t="s">
+      <c r="E115" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="F115" s="130"/>
-      <c r="G115" s="77"/>
-      <c r="H115" s="80"/>
-      <c r="I115" s="39"/>
-      <c r="J115" s="39"/>
-      <c r="K115" s="39"/>
-      <c r="L115" s="39"/>
-      <c r="M115" s="39"/>
-      <c r="N115" s="39"/>
+      <c r="F115" s="29" t="e">
+        <f>IF(OR(H115 = "", H115 = "ー", H115 = "-"), "", LOWER(H115) &amp; IF(N115 &lt;&gt; "", ":" &amp; N115 &amp; "|", "|") &amp; IF(O115 &lt;&gt; "", "search|", "")) &amp; "ja:" &amp;#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G115" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="H115" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="I115" s="30"/>
+      <c r="J115" s="30"/>
+      <c r="K115" s="30"/>
+      <c r="L115" s="30"/>
+      <c r="M115" s="30"/>
+      <c r="N115" s="30"/>
       <c r="O115" s="13"/>
       <c r="P115" s="31"/>
       <c r="Q115" s="21"/>
@@ -36694,33 +36725,28 @@
       <c r="AA115" s="12"/>
       <c r="AB115" s="12"/>
     </row>
-    <row r="116" spans="1:28" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="84">
+    <row r="116" spans="1:28" ht="18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="47">
         <v>2</v>
       </c>
-      <c r="B116" s="85"/>
-      <c r="C116" s="74" t="s">
-        <v>157</v>
-      </c>
-      <c r="D116" s="73" t="s">
-        <v>51</v>
-      </c>
-      <c r="E116" s="83" t="s">
-        <v>55</v>
-      </c>
-      <c r="F116" s="130" t="s">
-        <v>158</v>
-      </c>
-      <c r="G116" s="77"/>
-      <c r="H116" s="80"/>
-      <c r="I116" s="39"/>
-      <c r="J116" s="39"/>
-      <c r="K116" s="39"/>
-      <c r="L116" s="39"/>
-      <c r="M116" s="39"/>
-      <c r="N116" s="39"/>
-      <c r="O116" s="13"/>
-      <c r="P116" s="31"/>
+      <c r="B116" s="26"/>
+      <c r="C116" s="33"/>
+      <c r="D116" s="34"/>
+      <c r="E116" s="38"/>
+      <c r="F116" s="29" t="e">
+        <f>IF(OR(H116 = "", H116 = "ー", H116 = "-"), "", LOWER(H116) &amp; IF(N116 &lt;&gt; "", ":" &amp; N116 &amp; "|", "|") &amp; IF(O116 &lt;&gt; "", "search|", "")) &amp; "ja:" &amp;#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G116" s="28"/>
+      <c r="H116" s="30"/>
+      <c r="I116" s="30"/>
+      <c r="J116" s="30"/>
+      <c r="K116" s="30"/>
+      <c r="L116" s="30"/>
+      <c r="M116" s="30"/>
+      <c r="N116" s="30"/>
+      <c r="O116" s="28"/>
+      <c r="P116" s="36"/>
       <c r="Q116" s="21"/>
       <c r="R116" s="13"/>
       <c r="S116" s="13"/>
@@ -36734,33 +36760,28 @@
       <c r="AA116" s="12"/>
       <c r="AB116" s="12"/>
     </row>
-    <row r="117" spans="1:28" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="84">
+    <row r="117" spans="1:28" ht="18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="47">
         <v>3</v>
       </c>
-      <c r="B117" s="85"/>
-      <c r="C117" s="74" t="s">
-        <v>159</v>
-      </c>
-      <c r="D117" s="73" t="s">
-        <v>51</v>
-      </c>
-      <c r="E117" s="83" t="s">
-        <v>55</v>
-      </c>
-      <c r="F117" s="130" t="s">
-        <v>160</v>
-      </c>
-      <c r="G117" s="77"/>
-      <c r="H117" s="80"/>
-      <c r="I117" s="39"/>
-      <c r="J117" s="39"/>
-      <c r="K117" s="39"/>
-      <c r="L117" s="39"/>
-      <c r="M117" s="39"/>
-      <c r="N117" s="39"/>
-      <c r="O117" s="13"/>
-      <c r="P117" s="31"/>
+      <c r="B117" s="26"/>
+      <c r="C117" s="33"/>
+      <c r="D117" s="34"/>
+      <c r="E117" s="38"/>
+      <c r="F117" s="29" t="e">
+        <f>IF(OR(H117 = "", H117 = "ー", H117 = "-"), "", LOWER(H117) &amp; IF(N117 &lt;&gt; "", ":" &amp; N117 &amp; "|", "|") &amp; IF(O117 &lt;&gt; "", "search|", "")) &amp; "ja:" &amp;#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G117" s="28"/>
+      <c r="H117" s="30"/>
+      <c r="I117" s="30"/>
+      <c r="J117" s="30"/>
+      <c r="K117" s="30"/>
+      <c r="L117" s="30"/>
+      <c r="M117" s="30"/>
+      <c r="N117" s="30"/>
+      <c r="O117" s="28"/>
+      <c r="P117" s="36"/>
       <c r="Q117" s="21"/>
       <c r="R117" s="13"/>
       <c r="S117" s="13"/>
@@ -36774,33 +36795,28 @@
       <c r="AA117" s="12"/>
       <c r="AB117" s="12"/>
     </row>
-    <row r="118" spans="1:28" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="84">
+    <row r="118" spans="1:28" ht="18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="47">
         <v>4</v>
       </c>
-      <c r="B118" s="85"/>
-      <c r="C118" s="74" t="s">
-        <v>161</v>
-      </c>
-      <c r="D118" s="73" t="s">
-        <v>54</v>
-      </c>
-      <c r="E118" s="83" t="s">
-        <v>55</v>
-      </c>
-      <c r="F118" s="130" t="s">
-        <v>162</v>
-      </c>
-      <c r="G118" s="77"/>
-      <c r="H118" s="80"/>
-      <c r="I118" s="39"/>
-      <c r="J118" s="39"/>
-      <c r="K118" s="39"/>
-      <c r="L118" s="39"/>
-      <c r="M118" s="39"/>
-      <c r="N118" s="39"/>
-      <c r="O118" s="13"/>
-      <c r="P118" s="31"/>
+      <c r="B118" s="26"/>
+      <c r="C118" s="33"/>
+      <c r="D118" s="34"/>
+      <c r="E118" s="38"/>
+      <c r="F118" s="29" t="e">
+        <f>IF(OR(H118 = "", H118 = "ー", H118 = "-"), "", LOWER(H118) &amp; IF(N118 &lt;&gt; "", ":" &amp; N118 &amp; "|", "|") &amp; IF(O118 &lt;&gt; "", "search|", "")) &amp; "ja:" &amp;#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G118" s="28"/>
+      <c r="H118" s="30"/>
+      <c r="I118" s="48"/>
+      <c r="J118" s="48"/>
+      <c r="K118" s="48"/>
+      <c r="L118" s="48"/>
+      <c r="M118" s="48"/>
+      <c r="N118" s="48"/>
+      <c r="O118" s="28"/>
+      <c r="P118" s="36"/>
       <c r="Q118" s="21"/>
       <c r="R118" s="13"/>
       <c r="S118" s="13"/>
@@ -36814,23 +36830,26 @@
       <c r="AA118" s="12"/>
       <c r="AB118" s="12"/>
     </row>
-    <row r="119" spans="1:28" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="84"/>
-      <c r="B119" s="85"/>
-      <c r="C119" s="74"/>
-      <c r="D119" s="73"/>
-      <c r="E119" s="83"/>
-      <c r="F119" s="130"/>
-      <c r="G119" s="77"/>
-      <c r="H119" s="80"/>
-      <c r="I119" s="39"/>
-      <c r="J119" s="39"/>
-      <c r="K119" s="39"/>
-      <c r="L119" s="39"/>
-      <c r="M119" s="39"/>
-      <c r="N119" s="39"/>
+    <row r="119" spans="1:28" ht="18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="25"/>
+      <c r="B119" s="26"/>
+      <c r="C119" s="49"/>
+      <c r="D119" s="28"/>
+      <c r="E119" s="34"/>
+      <c r="F119" s="29" t="e">
+        <f>IF(OR(H119 = "", H119 = "ー", H119 = "-"), "", LOWER(H119) &amp; IF(N119 &lt;&gt; "", ":" &amp; N119 &amp; "|", "|") &amp; IF(O119 &lt;&gt; "", "search|", "")) &amp; "ja:" &amp;#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G119" s="28"/>
+      <c r="H119" s="30"/>
+      <c r="I119" s="30"/>
+      <c r="J119" s="30"/>
+      <c r="K119" s="30"/>
+      <c r="L119" s="30"/>
+      <c r="M119" s="30"/>
+      <c r="N119" s="30"/>
       <c r="O119" s="13"/>
-      <c r="P119" s="31"/>
+      <c r="P119" s="36"/>
       <c r="Q119" s="21"/>
       <c r="R119" s="13"/>
       <c r="S119" s="13"/>
@@ -36844,31 +36863,35 @@
       <c r="AA119" s="12"/>
       <c r="AB119" s="12"/>
     </row>
-    <row r="120" spans="1:28" s="115" customFormat="1" ht="31" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="88"/>
-      <c r="B120" s="89"/>
-      <c r="C120" s="89"/>
-      <c r="D120" s="89"/>
-      <c r="E120" s="89"/>
-      <c r="F120" s="90"/>
-      <c r="G120" s="89"/>
-      <c r="H120" s="89"/>
-      <c r="I120" s="89"/>
-      <c r="J120" s="89"/>
-      <c r="K120" s="89"/>
-      <c r="L120" s="89"/>
-      <c r="M120" s="89"/>
-      <c r="N120" s="89"/>
-      <c r="O120" s="89"/>
-      <c r="P120" s="134"/>
-    </row>
-    <row r="121" spans="1:28" s="76" customFormat="1" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="137"/>
-      <c r="B121" s="138"/>
-      <c r="C121" s="139"/>
-      <c r="D121" s="140"/>
-      <c r="E121" s="138"/>
-      <c r="F121" s="139"/>
+    <row r="120" spans="1:28" ht="14" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="60"/>
+      <c r="B120" s="61"/>
+      <c r="C120" s="61"/>
+      <c r="D120" s="61"/>
+      <c r="E120" s="61"/>
+      <c r="F120" s="62"/>
+      <c r="G120" s="61"/>
+      <c r="H120" s="61"/>
+      <c r="I120" s="61"/>
+      <c r="J120" s="61"/>
+      <c r="K120" s="61"/>
+      <c r="L120" s="61"/>
+      <c r="M120" s="61"/>
+      <c r="N120" s="61"/>
+      <c r="O120" s="61"/>
+      <c r="P120" s="64"/>
+    </row>
+    <row r="121" spans="1:28" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="144" t="s">
+        <v>155</v>
+      </c>
+      <c r="B121" s="140"/>
+      <c r="C121" s="141"/>
+      <c r="D121" s="156" t="s">
+        <v>156</v>
+      </c>
+      <c r="E121" s="140"/>
+      <c r="F121" s="141"/>
       <c r="G121" s="66"/>
       <c r="H121" s="66"/>
       <c r="I121" s="65"/>
@@ -36892,7 +36915,7 @@
       <c r="AA121" s="12"/>
       <c r="AB121" s="12"/>
     </row>
-    <row r="122" spans="1:28" s="131" customFormat="1" ht="29" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:28" ht="29" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A122" s="84">
         <v>1</v>
       </c>
@@ -36934,15 +36957,23 @@
       <c r="AA122" s="12"/>
       <c r="AB122" s="12"/>
     </row>
-    <row r="123" spans="1:28" s="131" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:28" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A123" s="84">
         <v>2</v>
       </c>
       <c r="B123" s="85"/>
-      <c r="C123" s="74"/>
-      <c r="D123" s="73"/>
-      <c r="E123" s="83"/>
-      <c r="F123" s="130"/>
+      <c r="C123" s="74" t="s">
+        <v>157</v>
+      </c>
+      <c r="D123" s="73" t="s">
+        <v>51</v>
+      </c>
+      <c r="E123" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="F123" s="130" t="s">
+        <v>158</v>
+      </c>
       <c r="G123" s="77"/>
       <c r="H123" s="80"/>
       <c r="I123" s="39"/>
@@ -36966,15 +36997,23 @@
       <c r="AA123" s="12"/>
       <c r="AB123" s="12"/>
     </row>
-    <row r="124" spans="1:28" s="131" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:28" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A124" s="84">
         <v>3</v>
       </c>
       <c r="B124" s="85"/>
-      <c r="C124" s="74"/>
-      <c r="D124" s="73"/>
-      <c r="E124" s="83"/>
-      <c r="F124" s="130"/>
+      <c r="C124" s="74" t="s">
+        <v>159</v>
+      </c>
+      <c r="D124" s="73" t="s">
+        <v>51</v>
+      </c>
+      <c r="E124" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="F124" s="130" t="s">
+        <v>160</v>
+      </c>
       <c r="G124" s="77"/>
       <c r="H124" s="80"/>
       <c r="I124" s="39"/>
@@ -36998,15 +37037,23 @@
       <c r="AA124" s="12"/>
       <c r="AB124" s="12"/>
     </row>
-    <row r="125" spans="1:28" s="131" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:28" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A125" s="84">
         <v>4</v>
       </c>
       <c r="B125" s="85"/>
-      <c r="C125" s="74"/>
-      <c r="D125" s="73"/>
-      <c r="E125" s="83"/>
-      <c r="F125" s="130"/>
+      <c r="C125" s="74" t="s">
+        <v>161</v>
+      </c>
+      <c r="D125" s="73" t="s">
+        <v>54</v>
+      </c>
+      <c r="E125" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="F125" s="130" t="s">
+        <v>162</v>
+      </c>
       <c r="G125" s="77"/>
       <c r="H125" s="80"/>
       <c r="I125" s="39"/>
@@ -37030,7 +37077,7 @@
       <c r="AA125" s="12"/>
       <c r="AB125" s="12"/>
     </row>
-    <row r="126" spans="1:28" s="131" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:28" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A126" s="84"/>
       <c r="B126" s="85"/>
       <c r="C126" s="74"/>
@@ -37078,13 +37125,13 @@
       <c r="O127" s="89"/>
       <c r="P127" s="134"/>
     </row>
-    <row r="128" spans="1:28" s="131" customFormat="1" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="137"/>
-      <c r="B128" s="138"/>
-      <c r="C128" s="139"/>
-      <c r="D128" s="140"/>
-      <c r="E128" s="138"/>
-      <c r="F128" s="139"/>
+    <row r="128" spans="1:28" s="76" customFormat="1" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="144"/>
+      <c r="B128" s="140"/>
+      <c r="C128" s="141"/>
+      <c r="D128" s="156"/>
+      <c r="E128" s="140"/>
+      <c r="F128" s="141"/>
       <c r="G128" s="66"/>
       <c r="H128" s="66"/>
       <c r="I128" s="65"/>
@@ -37294,28 +37341,223 @@
       <c r="O134" s="89"/>
       <c r="P134" s="134"/>
     </row>
-    <row r="135" spans="1:28" ht="14" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="F135" s="68"/>
-    </row>
-    <row r="136" spans="1:28" ht="13" x14ac:dyDescent="0.15">
-      <c r="F136" s="68"/>
-    </row>
-    <row r="137" spans="1:28" ht="13" x14ac:dyDescent="0.15">
-      <c r="F137" s="68"/>
-    </row>
-    <row r="138" spans="1:28" ht="13" x14ac:dyDescent="0.15">
-      <c r="F138" s="68"/>
-    </row>
-    <row r="139" spans="1:28" ht="13" x14ac:dyDescent="0.15">
-      <c r="F139" s="68"/>
-    </row>
-    <row r="140" spans="1:28" ht="13" x14ac:dyDescent="0.15">
-      <c r="F140" s="68"/>
-    </row>
-    <row r="141" spans="1:28" ht="13" x14ac:dyDescent="0.15">
-      <c r="F141" s="68"/>
-    </row>
-    <row r="142" spans="1:28" ht="13" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:28" s="131" customFormat="1" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="144"/>
+      <c r="B135" s="140"/>
+      <c r="C135" s="141"/>
+      <c r="D135" s="156"/>
+      <c r="E135" s="140"/>
+      <c r="F135" s="141"/>
+      <c r="G135" s="66"/>
+      <c r="H135" s="66"/>
+      <c r="I135" s="65"/>
+      <c r="J135" s="65"/>
+      <c r="K135" s="65"/>
+      <c r="L135" s="65"/>
+      <c r="M135" s="65"/>
+      <c r="N135" s="65"/>
+      <c r="O135" s="66"/>
+      <c r="P135" s="67"/>
+      <c r="Q135" s="21"/>
+      <c r="R135" s="12"/>
+      <c r="S135" s="12"/>
+      <c r="T135" s="12"/>
+      <c r="U135" s="12"/>
+      <c r="V135" s="12"/>
+      <c r="W135" s="12"/>
+      <c r="X135" s="12"/>
+      <c r="Y135" s="12"/>
+      <c r="Z135" s="12"/>
+      <c r="AA135" s="12"/>
+      <c r="AB135" s="12"/>
+    </row>
+    <row r="136" spans="1:28" s="131" customFormat="1" ht="29" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="84">
+        <v>1</v>
+      </c>
+      <c r="B136" s="85" t="s">
+        <v>46</v>
+      </c>
+      <c r="C136" s="74" t="s">
+        <v>47</v>
+      </c>
+      <c r="D136" s="73" t="s">
+        <v>48</v>
+      </c>
+      <c r="E136" s="83" t="s">
+        <v>49</v>
+      </c>
+      <c r="F136" s="130"/>
+      <c r="G136" s="77"/>
+      <c r="H136" s="80"/>
+      <c r="I136" s="39"/>
+      <c r="J136" s="39"/>
+      <c r="K136" s="39"/>
+      <c r="L136" s="39"/>
+      <c r="M136" s="39"/>
+      <c r="N136" s="39"/>
+      <c r="O136" s="13"/>
+      <c r="P136" s="31"/>
+      <c r="Q136" s="21"/>
+      <c r="R136" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="S136" s="13"/>
+      <c r="T136" s="13"/>
+      <c r="U136" s="13"/>
+      <c r="V136" s="13"/>
+      <c r="W136" s="13"/>
+      <c r="X136" s="12"/>
+      <c r="Y136" s="12"/>
+      <c r="Z136" s="12"/>
+      <c r="AA136" s="12"/>
+      <c r="AB136" s="12"/>
+    </row>
+    <row r="137" spans="1:28" s="131" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="84">
+        <v>2</v>
+      </c>
+      <c r="B137" s="85"/>
+      <c r="C137" s="74"/>
+      <c r="D137" s="73"/>
+      <c r="E137" s="83"/>
+      <c r="F137" s="130"/>
+      <c r="G137" s="77"/>
+      <c r="H137" s="80"/>
+      <c r="I137" s="39"/>
+      <c r="J137" s="39"/>
+      <c r="K137" s="39"/>
+      <c r="L137" s="39"/>
+      <c r="M137" s="39"/>
+      <c r="N137" s="39"/>
+      <c r="O137" s="13"/>
+      <c r="P137" s="31"/>
+      <c r="Q137" s="21"/>
+      <c r="R137" s="13"/>
+      <c r="S137" s="13"/>
+      <c r="T137" s="13"/>
+      <c r="U137" s="13"/>
+      <c r="V137" s="13"/>
+      <c r="W137" s="13"/>
+      <c r="X137" s="12"/>
+      <c r="Y137" s="12"/>
+      <c r="Z137" s="12"/>
+      <c r="AA137" s="12"/>
+      <c r="AB137" s="12"/>
+    </row>
+    <row r="138" spans="1:28" s="131" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="84">
+        <v>3</v>
+      </c>
+      <c r="B138" s="85"/>
+      <c r="C138" s="74"/>
+      <c r="D138" s="73"/>
+      <c r="E138" s="83"/>
+      <c r="F138" s="130"/>
+      <c r="G138" s="77"/>
+      <c r="H138" s="80"/>
+      <c r="I138" s="39"/>
+      <c r="J138" s="39"/>
+      <c r="K138" s="39"/>
+      <c r="L138" s="39"/>
+      <c r="M138" s="39"/>
+      <c r="N138" s="39"/>
+      <c r="O138" s="13"/>
+      <c r="P138" s="31"/>
+      <c r="Q138" s="21"/>
+      <c r="R138" s="13"/>
+      <c r="S138" s="13"/>
+      <c r="T138" s="13"/>
+      <c r="U138" s="13"/>
+      <c r="V138" s="13"/>
+      <c r="W138" s="13"/>
+      <c r="X138" s="12"/>
+      <c r="Y138" s="12"/>
+      <c r="Z138" s="12"/>
+      <c r="AA138" s="12"/>
+      <c r="AB138" s="12"/>
+    </row>
+    <row r="139" spans="1:28" s="131" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="84">
+        <v>4</v>
+      </c>
+      <c r="B139" s="85"/>
+      <c r="C139" s="74"/>
+      <c r="D139" s="73"/>
+      <c r="E139" s="83"/>
+      <c r="F139" s="130"/>
+      <c r="G139" s="77"/>
+      <c r="H139" s="80"/>
+      <c r="I139" s="39"/>
+      <c r="J139" s="39"/>
+      <c r="K139" s="39"/>
+      <c r="L139" s="39"/>
+      <c r="M139" s="39"/>
+      <c r="N139" s="39"/>
+      <c r="O139" s="13"/>
+      <c r="P139" s="31"/>
+      <c r="Q139" s="21"/>
+      <c r="R139" s="13"/>
+      <c r="S139" s="13"/>
+      <c r="T139" s="13"/>
+      <c r="U139" s="13"/>
+      <c r="V139" s="13"/>
+      <c r="W139" s="13"/>
+      <c r="X139" s="12"/>
+      <c r="Y139" s="12"/>
+      <c r="Z139" s="12"/>
+      <c r="AA139" s="12"/>
+      <c r="AB139" s="12"/>
+    </row>
+    <row r="140" spans="1:28" s="131" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="84"/>
+      <c r="B140" s="85"/>
+      <c r="C140" s="74"/>
+      <c r="D140" s="73"/>
+      <c r="E140" s="83"/>
+      <c r="F140" s="130"/>
+      <c r="G140" s="77"/>
+      <c r="H140" s="80"/>
+      <c r="I140" s="39"/>
+      <c r="J140" s="39"/>
+      <c r="K140" s="39"/>
+      <c r="L140" s="39"/>
+      <c r="M140" s="39"/>
+      <c r="N140" s="39"/>
+      <c r="O140" s="13"/>
+      <c r="P140" s="31"/>
+      <c r="Q140" s="21"/>
+      <c r="R140" s="13"/>
+      <c r="S140" s="13"/>
+      <c r="T140" s="13"/>
+      <c r="U140" s="13"/>
+      <c r="V140" s="13"/>
+      <c r="W140" s="13"/>
+      <c r="X140" s="12"/>
+      <c r="Y140" s="12"/>
+      <c r="Z140" s="12"/>
+      <c r="AA140" s="12"/>
+      <c r="AB140" s="12"/>
+    </row>
+    <row r="141" spans="1:28" s="115" customFormat="1" ht="31" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="88"/>
+      <c r="B141" s="89"/>
+      <c r="C141" s="89"/>
+      <c r="D141" s="89"/>
+      <c r="E141" s="89"/>
+      <c r="F141" s="90"/>
+      <c r="G141" s="89"/>
+      <c r="H141" s="89"/>
+      <c r="I141" s="89"/>
+      <c r="J141" s="89"/>
+      <c r="K141" s="89"/>
+      <c r="L141" s="89"/>
+      <c r="M141" s="89"/>
+      <c r="N141" s="89"/>
+      <c r="O141" s="89"/>
+      <c r="P141" s="134"/>
+    </row>
+    <row r="142" spans="1:28" ht="14" thickTop="1" x14ac:dyDescent="0.15">
       <c r="F142" s="68"/>
     </row>
     <row r="143" spans="1:28" ht="13" x14ac:dyDescent="0.15">
@@ -40117,14 +40359,43 @@
     <row r="1075" spans="6:6" ht="13" x14ac:dyDescent="0.15">
       <c r="F1075" s="68"/>
     </row>
+    <row r="1076" spans="6:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="F1076" s="68"/>
+    </row>
+    <row r="1077" spans="6:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="F1077" s="68"/>
+    </row>
+    <row r="1078" spans="6:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="F1078" s="68"/>
+    </row>
+    <row r="1079" spans="6:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="F1079" s="68"/>
+    </row>
+    <row r="1080" spans="6:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="F1080" s="68"/>
+    </row>
+    <row r="1081" spans="6:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="F1081" s="68"/>
+    </row>
+    <row r="1082" spans="6:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="F1082" s="68"/>
+    </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="A135:C135"/>
+    <mergeCell ref="D135:F135"/>
+    <mergeCell ref="D114:F114"/>
+    <mergeCell ref="D64:F64"/>
+    <mergeCell ref="A121:C121"/>
+    <mergeCell ref="D121:F121"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="A89:C89"/>
+    <mergeCell ref="D89:F89"/>
+    <mergeCell ref="A104:C104"/>
+    <mergeCell ref="D104:F104"/>
+    <mergeCell ref="A128:C128"/>
+    <mergeCell ref="D128:F128"/>
+    <mergeCell ref="A114:C114"/>
     <mergeCell ref="R1:W1"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A3:C3"/>
@@ -40132,20 +40403,12 @@
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="G1:O1"/>
-    <mergeCell ref="A128:C128"/>
-    <mergeCell ref="D128:F128"/>
-    <mergeCell ref="D107:F107"/>
-    <mergeCell ref="D64:F64"/>
-    <mergeCell ref="A114:C114"/>
-    <mergeCell ref="D114:F114"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="A82:C82"/>
-    <mergeCell ref="D82:F82"/>
-    <mergeCell ref="A97:C97"/>
-    <mergeCell ref="D97:F97"/>
-    <mergeCell ref="A121:C121"/>
-    <mergeCell ref="D121:F121"/>
-    <mergeCell ref="A107:C107"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="D54:F54"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>